<commit_message>
Añado una parte del pto. 4 del pdp
</commit_message>
<xml_diff>
--- a/Tabla_EDT_0.9.xlsx
+++ b/Tabla_EDT_0.9.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OTI\Documents\Uni_Data\IS\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youss\Documents\LaCompannia\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B076A6DD-204E-4AA8-A7B1-56320157B262}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -99,28 +100,6 @@
   </si>
   <si>
     <t>Daniel Alfaro Miranda</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Luis Pozas Palomo   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
   </si>
   <si>
     <t>Mingyang Chen</t>
@@ -681,12 +660,34 @@
    -20/03/18
    -(…)</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Luis Pozas Palomo   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,29 +696,69 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -725,50 +766,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1049,600 +1137,608 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="25.28515625" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" customWidth="1"/>
+    <col min="9" max="9" width="27.44140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" customWidth="1"/>
+    <col min="11" max="11" width="26.44140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" customWidth="1"/>
+    <col min="13" max="13" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="22"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="23"/>
+      <c r="F2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="23"/>
+      <c r="I2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="11"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+    </row>
+    <row r="5" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+    </row>
+    <row r="7" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" s="27"/>
+    </row>
+    <row r="8" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+    </row>
+    <row r="9" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="M9" s="27"/>
+    </row>
+    <row r="10" spans="1:13" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+    </row>
+    <row r="11" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="M11" s="27"/>
+    </row>
+    <row r="12" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+    </row>
+    <row r="13" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="M13" s="27"/>
+    </row>
+    <row r="14" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+    </row>
+    <row r="15" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="M15" s="27"/>
+    </row>
+    <row r="16" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+    </row>
+    <row r="17" spans="1:13" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="M17" s="27"/>
+    </row>
+    <row r="18" spans="1:13" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+    </row>
+    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="24"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="2" t="s">
+      <c r="B21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="D21" s="26"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="M3" s="12" t="s">
+      <c r="C22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+    </row>
+    <row r="24" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-    </row>
-    <row r="5" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="H5" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="M5" s="14"/>
-    </row>
-    <row r="6" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="H7" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="H9" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:13" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="H11" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="H13" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="M13" s="14"/>
-    </row>
-    <row r="14" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="H15" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-    </row>
-    <row r="17" spans="1:13" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="12" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="1:13" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+    </row>
+    <row r="26" spans="1:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="H17" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="M17" s="14"/>
-    </row>
-    <row r="18" spans="1:13" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:13" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-    </row>
-    <row r="24" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-    </row>
-    <row r="25" spans="1:13" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="8" t="s">
+      <c r="D26" s="21"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+    </row>
+    <row r="27" spans="1:13" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-    </row>
-    <row r="26" spans="1:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-    </row>
-    <row r="27" spans="1:13" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="D27" s="21"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+    </row>
+    <row r="28" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="8" t="s">
+      <c r="B28" s="20"/>
+      <c r="C28" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-    </row>
-    <row r="28" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-    </row>
-    <row r="29" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="D28" s="21"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+    </row>
+    <row r="29" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="59">
@@ -1677,20 +1773,12 @@
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="H17:H18"/>
+    <mergeCell ref="D11:D12"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="I3:I18"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B22:B29"/>
-    <mergeCell ref="D22:D29"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F3:F18"/>
@@ -1703,8 +1791,16 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
     <mergeCell ref="B3:B18"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="D22:D29"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>